<commit_message>
Addition of LH in PL
</commit_message>
<xml_diff>
--- a/images/projects/Project List.xlsx
+++ b/images/projects/Project List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Rattan Raj Trinity Rudra</t>
+  </si>
+  <si>
+    <t>Landscape Heritage</t>
   </si>
 </sst>
 </file>
@@ -228,7 +231,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -251,11 +254,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -269,6 +283,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -572,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,7 +776,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="4">
-        <v>43070</v>
+        <v>43435</v>
       </c>
       <c r="F7" s="1">
         <v>140</v>
@@ -1225,6 +1242,29 @@
       </c>
       <c r="H26" s="1" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="4">
+        <v>44166</v>
+      </c>
+      <c r="F27" s="7">
+        <v>250</v>
+      </c>
+      <c r="G27" s="7">
+        <v>24</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>